<commit_message>
Chnages for req, diagnostics
</commit_message>
<xml_diff>
--- a/doc/voice_to_text_requirements.xlsx
+++ b/doc/voice_to_text_requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91843\RWUVT\RWVT\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\108449\Downloads\personal\dev\RWVT\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21222C40-716A-40F9-AD38-A0B48BCFD3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CF5D56-9909-44D1-BC6F-4FF57196439E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="828" windowWidth="23040" windowHeight="11412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>System</t>
   </si>
@@ -46,113 +46,62 @@
     <t>Voice-to-Text</t>
   </si>
   <si>
-    <t>RWS00001</t>
-  </si>
-  <si>
-    <t>RWS00002</t>
-  </si>
-  <si>
-    <t>RWS00003</t>
-  </si>
-  <si>
-    <t>RWS00004</t>
-  </si>
-  <si>
-    <t>RWS00005</t>
-  </si>
-  <si>
-    <t>RWS00006</t>
-  </si>
-  <si>
-    <t>RWS00007</t>
-  </si>
-  <si>
-    <t>RWS00008</t>
-  </si>
-  <si>
-    <t>RWS00009</t>
-  </si>
-  <si>
-    <t>RWS00010</t>
-  </si>
-  <si>
-    <t>RWS00011</t>
-  </si>
-  <si>
-    <t>RWS00012</t>
-  </si>
-  <si>
-    <t>RWS00013</t>
-  </si>
-  <si>
-    <t>RWS00014</t>
-  </si>
-  <si>
-    <t>RWS00015</t>
-  </si>
-  <si>
-    <t>RWS00016</t>
-  </si>
-  <si>
-    <t>RWS00017</t>
-  </si>
-  <si>
-    <t>The system should test function name.</t>
-  </si>
-  <si>
-    <t>The system should test audio file argument.</t>
-  </si>
-  <si>
-    <t>The system should test wav format support.</t>
-  </si>
-  <si>
-    <t>The system should test mp3 format support.</t>
-  </si>
-  <si>
-    <t>The system should test unsupported format.</t>
-  </si>
-  <si>
-    <t>The system should test invalid audio file.</t>
-  </si>
-  <si>
-    <t>The system should test empty audio file.</t>
-  </si>
-  <si>
-    <t>The system should test speech recognition output.</t>
-  </si>
-  <si>
-    <t>The system should test background noise handling.</t>
-  </si>
-  <si>
-    <t>The system should test multiple speakers.</t>
-  </si>
-  <si>
-    <t>The system should test long audio file.</t>
-  </si>
-  <si>
-    <t>The system should test short audio file.</t>
-  </si>
-  <si>
-    <t>The system should test special characters.</t>
-  </si>
-  <si>
-    <t>The system should test accuracy with accents.</t>
-  </si>
-  <si>
-    <t>The system should test punctuation handling.</t>
-  </si>
-  <si>
-    <t>The system should test response format.</t>
-  </si>
-  <si>
-    <t>The system should test logging.</t>
+    <t>RWVT00001</t>
+  </si>
+  <si>
+    <t>RWVT00002</t>
+  </si>
+  <si>
+    <t>RWVT00003</t>
+  </si>
+  <si>
+    <t>RWVT00004</t>
+  </si>
+  <si>
+    <t>RWVT00005</t>
+  </si>
+  <si>
+    <t>RWVT00006</t>
+  </si>
+  <si>
+    <t>RWVT00007</t>
+  </si>
+  <si>
+    <t>RWVT00008</t>
+  </si>
+  <si>
+    <t>function should be voice_to_text()</t>
+  </si>
+  <si>
+    <t>Input argument must be JSON</t>
+  </si>
+  <si>
+    <t>the JSON object must contain audio file data, which will be processed by the respective voice-to-text service.</t>
+  </si>
+  <si>
+    <t>Return argument must for JSON</t>
+  </si>
+  <si>
+    <t>Return object for JSON have comprised with following
+a. status: SUCCESS/ERROR
+b. error: AUDIO_ERROR/API_ERROR/SERVER_BUSY/UNDEFINED
+c. response: the transcribed text from the voice-to-text service</t>
+  </si>
+  <si>
+    <t>the function should establish a connection with a Google voice-to-text service and process the given audio data.</t>
+  </si>
+  <si>
+    <t>once the connection is established, the function should send the audio data to the service and retrieve the text response.</t>
+  </si>
+  <si>
+    <t>The function must return the JSON object with the transcribed text and relevant status/error details, as specified in RWS00005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +113,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -223,6 +178,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +489,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,7 +497,7 @@
     <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="50.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -574,7 +532,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -585,7 +543,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -596,7 +554,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -607,18 +565,18 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
-        <v>29</v>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -629,7 +587,7 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -640,7 +598,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -651,107 +609,53 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" t="s">
-        <v>41</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -759,6 +663,7 @@
     <mergeCell ref="B2:B18"/>
     <mergeCell ref="A2:A18"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>